<commit_message>
Write part data to excel spreadsheet
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -4,57 +4,18 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="23640"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="23640"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Info" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:O76"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
-  <si>
-    <t>tp01</t>
-  </si>
-  <si>
-    <t>Gopal</t>
-  </si>
-  <si>
-    <t>Technical Manager</t>
-  </si>
-  <si>
-    <t>tp02</t>
-  </si>
-  <si>
-    <t>Proof Reader</t>
-  </si>
-  <si>
-    <t>tp03</t>
-  </si>
-  <si>
-    <t>Masthan</t>
-  </si>
-  <si>
-    <t>Technical Writer</t>
-  </si>
-  <si>
-    <t>tp04</t>
-  </si>
-  <si>
-    <t>tp05</t>
-  </si>
-  <si>
-    <t>Krishna</t>
-  </si>
-  <si>
-    <t>sdfgsdgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgfgf</t>
-  </si>
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>PART NAME</t>
   </si>
@@ -72,14 +33,31 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>Sprocket</t>
+  </si>
+  <si>
+    <t>Carlingview</t>
+  </si>
+  <si>
+    <t>4568794231</t>
+  </si>
+  <si>
+    <t>PLC Room</t>
+  </si>
+  <si>
+    <t>EN-23</t>
+  </si>
+  <si>
+    <t>45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -424,94 +402,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="43.85546875" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7109375" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.7109375" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="4.140625" collapsed="false"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new theme to interface and added back button to Add Part page
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>PART NAME</t>
   </si>
@@ -51,13 +51,44 @@
   </si>
   <si>
     <t>45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">too </t>
+  </si>
+  <si>
+    <t>cool</t>
+  </si>
+  <si>
+    <t>4987321</t>
+  </si>
+  <si>
+    <t>Mezzanine</t>
+  </si>
+  <si>
+    <t>EN-48</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>asf</t>
+  </si>
+  <si>
+    <t>qwe</t>
+  </si>
+  <si>
+    <t>a-q</t>
+  </si>
+  <si>
+    <t>qq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -410,11 +441,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="7.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -457,6 +488,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Search Part Frame now displays parts saved in excel sheet
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="104">
   <si>
     <t>PART NAME</t>
   </si>
@@ -81,6 +81,252 @@
   </si>
   <si>
     <t>qq</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>564987231321</t>
+  </si>
+  <si>
+    <t>Plant</t>
+  </si>
+  <si>
+    <t>EN-25</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>12341234</t>
+  </si>
+  <si>
+    <t>Electrical Room</t>
+  </si>
+  <si>
+    <t>en-12</t>
+  </si>
+  <si>
+    <t>212</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>banana</t>
+  </si>
+  <si>
+    <t>54987231</t>
+  </si>
+  <si>
+    <t>AS-78</t>
+  </si>
+  <si>
+    <t>216987987</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>645987</t>
+  </si>
+  <si>
+    <t>ew-59</t>
+  </si>
+  <si>
+    <t>654987</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>ae-12</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>897564312</t>
+  </si>
+  <si>
+    <t>Mezzanine Room</t>
+  </si>
+  <si>
+    <t>EN-12</t>
+  </si>
+  <si>
+    <t>897984</t>
+  </si>
+  <si>
+    <t>lol</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>1234123423</t>
+  </si>
+  <si>
+    <t>ev-23</t>
+  </si>
+  <si>
+    <t>987943251324586</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5-8</t>
+  </si>
+  <si>
+    <t>334</t>
+  </si>
+  <si>
+    <t>qw</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>h-3</t>
+  </si>
+  <si>
+    <t>h35h</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>23-44</t>
+  </si>
+  <si>
+    <t>2222222222222222222222222222222</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>sasssss</t>
+  </si>
+  <si>
+    <t>212334</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>qasdf</t>
+  </si>
+  <si>
+    <t>12341234-12341234</t>
+  </si>
+  <si>
+    <t>0000000000</t>
+  </si>
+  <si>
+    <t>00000000000</t>
+  </si>
+  <si>
+    <t>0-0</t>
+  </si>
+  <si>
+    <t>111111111</t>
+  </si>
+  <si>
+    <t>1111111111</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>111111111111</t>
+  </si>
+  <si>
+    <t>999999999</t>
+  </si>
+  <si>
+    <t>9999999</t>
+  </si>
+  <si>
+    <t>9-9</t>
+  </si>
+  <si>
+    <t>999999999999</t>
+  </si>
+  <si>
+    <t>444444444</t>
+  </si>
+  <si>
+    <t>44444444</t>
+  </si>
+  <si>
+    <t>44-4</t>
+  </si>
+  <si>
+    <t>444444</t>
+  </si>
+  <si>
+    <t>eightmonths</t>
+  </si>
+  <si>
+    <t>eightmonths-eightmonths</t>
+  </si>
+  <si>
+    <t>77777777777</t>
+  </si>
+  <si>
+    <t>7777777777777777777</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>77-77</t>
+  </si>
+  <si>
+    <t>7777777777777777</t>
+  </si>
+  <si>
+    <t>fantastic</t>
+  </si>
+  <si>
+    <t>fantastic-fantastic</t>
+  </si>
+  <si>
+    <t>asdf-asdf</t>
   </si>
 </sst>
 </file>
@@ -528,6 +774,426 @@
         <v>21</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Edit Part page, and enabled delete part.
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="23640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11955" windowHeight="23640"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Info" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="89">
   <si>
     <t>PART NAME</t>
   </si>
@@ -43,51 +43,15 @@
     <t>Sprocket</t>
   </si>
   <si>
-    <t>Carlingview</t>
-  </si>
-  <si>
-    <t>4568794231</t>
-  </si>
-  <si>
     <t>PLC Room</t>
   </si>
   <si>
-    <t>EN-23</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">too </t>
-  </si>
-  <si>
-    <t>cool</t>
-  </si>
-  <si>
-    <t>4987321</t>
-  </si>
-  <si>
     <t>Mezzanine</t>
   </si>
   <si>
-    <t>EN-48</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
-    <t>asf</t>
-  </si>
-  <si>
-    <t>qwe</t>
-  </si>
-  <si>
-    <t>a-q</t>
-  </si>
-  <si>
-    <t>qq</t>
-  </si>
-  <si>
     <t>Google</t>
   </si>
   <si>
@@ -97,9 +61,6 @@
     <t>Plant</t>
   </si>
   <si>
-    <t>EN-25</t>
-  </si>
-  <si>
     <t>46</t>
   </si>
   <si>
@@ -253,96 +214,9 @@
     <t>qasdf</t>
   </si>
   <si>
-    <t>12341234-12341234</t>
-  </si>
-  <si>
-    <t>0000000000</t>
-  </si>
-  <si>
-    <t>00000000000</t>
-  </si>
-  <si>
-    <t>0-0</t>
-  </si>
-  <si>
-    <t>111111111</t>
-  </si>
-  <si>
-    <t>1111111111</t>
-  </si>
-  <si>
-    <t>11111</t>
-  </si>
-  <si>
-    <t>1-1</t>
-  </si>
-  <si>
-    <t>111111111111</t>
-  </si>
-  <si>
-    <t>999999999</t>
-  </si>
-  <si>
-    <t>9999999</t>
-  </si>
-  <si>
-    <t>9-9</t>
-  </si>
-  <si>
-    <t>999999999999</t>
-  </si>
-  <si>
-    <t>444444444</t>
-  </si>
-  <si>
-    <t>44444444</t>
-  </si>
-  <si>
-    <t>44-4</t>
-  </si>
-  <si>
-    <t>444444</t>
-  </si>
-  <si>
     <t>eightmonths</t>
   </si>
   <si>
-    <t>eightmonths-eightmonths</t>
-  </si>
-  <si>
-    <t>77777777777</t>
-  </si>
-  <si>
-    <t>7777777777777777777</t>
-  </si>
-  <si>
-    <t>777</t>
-  </si>
-  <si>
-    <t>77-77</t>
-  </si>
-  <si>
-    <t>7777777777777777</t>
-  </si>
-  <si>
-    <t>fantastic</t>
-  </si>
-  <si>
-    <t>fantastic-fantastic</t>
-  </si>
-  <si>
-    <t>asdf-asdf</t>
-  </si>
-  <si>
-    <t>finally</t>
-  </si>
-  <si>
-    <t>fi-23</t>
-  </si>
-  <si>
-    <t>3223233</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -359,6 +233,60 @@
   </si>
   <si>
     <t>asdfasdf</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>23232323</t>
+  </si>
+  <si>
+    <t>toughtytatat</t>
+  </si>
+  <si>
+    <t>21341234</t>
+  </si>
+  <si>
+    <t>aa-22</t>
+  </si>
+  <si>
+    <t>2323</t>
+  </si>
+  <si>
+    <t>eightmonths in the year</t>
+  </si>
+  <si>
+    <t>probably</t>
+  </si>
+  <si>
+    <t>43431234</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>cc-cc</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>fsdg</t>
+  </si>
+  <si>
+    <t>sdfgsdfg</t>
+  </si>
+  <si>
+    <t>er-er</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>asdfasdfasdfasdfprobably</t>
   </si>
 </sst>
 </file>
@@ -711,10 +639,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,113 +679,113 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
         <v>31</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>34</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>35</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>36</v>
@@ -868,67 +796,67 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
         <v>52</v>
@@ -937,7 +865,7 @@
         <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
         <v>54</v>
@@ -957,30 +885,30 @@
         <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
         <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="F13" t="s">
         <v>64</v>
@@ -988,262 +916,102 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
         <v>71</v>
       </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
         <v>72</v>
       </c>
-      <c r="F15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F13" t="s">
         <v>80</v>
-      </c>
-      <c r="F18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" t="s">
-        <v>88</v>
-      </c>
-      <c r="F20" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" t="s">
-        <v>91</v>
-      </c>
-      <c r="C21" t="s">
-        <v>90</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>92</v>
-      </c>
-      <c r="F21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" t="s">
-        <v>97</v>
-      </c>
-      <c r="C23" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>101</v>
-      </c>
-      <c r="B24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" t="s">
-        <v>102</v>
-      </c>
-      <c r="F24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" t="s">
-        <v>52</v>
-      </c>
-      <c r="D25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" t="s">
-        <v>103</v>
-      </c>
-      <c r="F25" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" t="s">
-        <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" t="s">
-        <v>105</v>
-      </c>
-      <c r="F26" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1253,9 +1021,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B2:D4"/>
     </sheetView>
   </sheetViews>
@@ -1266,67 +1034,72 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>112</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restricted quantity field to only numbers. Enabled delete parts button
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -16,11 +16,12 @@
     <sheet name="Manufacturer" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t>PART NAME</t>
   </si>
@@ -85,9 +86,6 @@
     <t>apple</t>
   </si>
   <si>
-    <t>banana</t>
-  </si>
-  <si>
     <t>54987231</t>
   </si>
   <si>
@@ -184,36 +182,18 @@
     <t>13</t>
   </si>
   <si>
-    <t>23-44</t>
-  </si>
-  <si>
     <t>2222222222222222222222222222222</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>33</t>
-  </si>
-  <si>
     <t>44</t>
   </si>
   <si>
     <t>1-2</t>
   </si>
   <si>
-    <t>sasssss</t>
-  </si>
-  <si>
-    <t>212334</t>
-  </si>
-  <si>
-    <t>2-3</t>
-  </si>
-  <si>
-    <t>qasdf</t>
-  </si>
-  <si>
     <t>eightmonths</t>
   </si>
   <si>
@@ -265,61 +245,13 @@
     <t>43431234</t>
   </si>
   <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t>cc-cc</t>
-  </si>
-  <si>
-    <t>ccc</t>
-  </si>
-  <si>
-    <t>fsdg</t>
-  </si>
-  <si>
-    <t>sdfgsdfg</t>
-  </si>
-  <si>
-    <t>er-er</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>asdfasdfasdfasdfprobably</t>
-  </si>
-  <si>
-    <t>cccc</t>
-  </si>
-  <si>
-    <t>ccccccw</t>
-  </si>
-  <si>
-    <t>rr-rr</t>
-  </si>
-  <si>
-    <t>3333333</t>
-  </si>
-  <si>
     <t>,,,,,,,,,,/////////</t>
   </si>
   <si>
     <t>////p0</t>
   </si>
   <si>
-    <t>0-0-</t>
-  </si>
-  <si>
     <t>----</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         ddddddd</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>g-g</t>
   </si>
   <si>
     <t>23-4477</t>
@@ -678,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:F18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +650,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
@@ -727,7 +659,7 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -761,16 +693,16 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -778,19 +710,19 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
         <v>25</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
       </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -798,16 +730,16 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -815,302 +747,122 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>40</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
         <v>41</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
       </c>
       <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
         <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>78</v>
-      </c>
-      <c r="B13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
         <v>76</v>
-      </c>
-      <c r="F14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>79</v>
-      </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>98</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1133,42 +885,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -1178,27 +930,27 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Require description and identification before adding to database
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
   <si>
     <t>PART NAME</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>78-8888</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -845,6 +848,26 @@
         <v>76</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor and code cleanup
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="122">
   <si>
     <t>PART NAME</t>
   </si>
@@ -386,18 +386,6 @@
   </si>
   <si>
     <t>82SR0118, SR100</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>UPAK</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>SETTINGS</t>
   </si>
 </sst>
 </file>
@@ -2218,26 +2206,6 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>125</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added error message dialog and confirmation dialog
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -1918,33 +1918,33 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D59" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
       <c r="E59" t="s">
         <v>102</v>
       </c>
-      <c r="F59" t="n">
-        <v>4.0</v>
+      <c r="F59">
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
@@ -1953,18 +1953,18 @@
         <v>102</v>
       </c>
       <c r="F60">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
@@ -1978,13 +1978,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
@@ -1993,18 +1993,18 @@
         <v>102</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>109</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C63" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
@@ -2013,38 +2013,38 @@
         <v>102</v>
       </c>
       <c r="F63">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B64" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
       </c>
       <c r="E64" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="F64">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
@@ -2053,18 +2053,18 @@
         <v>114</v>
       </c>
       <c r="F65">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D66" t="s">
         <v>6</v>
@@ -2078,13 +2078,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>116</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D67" t="s">
         <v>6</v>
@@ -2093,26 +2093,6 @@
         <v>114</v>
       </c>
       <c r="F67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>12</v>
-      </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" t="s">
-        <v>118</v>
-      </c>
-      <c r="D68" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68" t="s">
-        <v>114</v>
-      </c>
-      <c r="F68">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactor and disable equipment textfield
</commit_message>
<xml_diff>
--- a/Parts/database.xlsx
+++ b/Parts/database.xlsx
@@ -1618,22 +1618,22 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
         <v>6</v>
       </c>
       <c r="E44" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F44">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,7 +1644,7 @@
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
         <v>6</v>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D46" t="s">
         <v>6</v>
@@ -1673,18 +1673,18 @@
         <v>78</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D47" t="s">
         <v>6</v>
@@ -1693,18 +1693,18 @@
         <v>78</v>
       </c>
       <c r="F47">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D48" t="s">
         <v>6</v>
@@ -1713,18 +1713,18 @@
         <v>78</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D49" t="s">
         <v>6</v>
@@ -1738,13 +1738,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
         <v>6</v>
@@ -1753,7 +1753,7 @@
         <v>78</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1764,16 +1764,16 @@
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D51" t="s">
         <v>6</v>
       </c>
       <c r="E51" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="F51">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1784,7 +1784,7 @@
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D52" t="s">
         <v>6</v>
@@ -1793,7 +1793,7 @@
         <v>92</v>
       </c>
       <c r="F52">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D53" t="s">
         <v>6</v>
@@ -1813,18 +1813,18 @@
         <v>92</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C54" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
@@ -1833,7 +1833,7 @@
         <v>92</v>
       </c>
       <c r="F54">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1844,7 +1844,7 @@
         <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -1858,13 +1858,13 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
@@ -1873,58 +1873,58 @@
         <v>92</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
       </c>
       <c r="E57" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F57">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>104</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
       </c>
       <c r="E58" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="F58">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D59" t="s">
         <v>6</v>
@@ -1933,18 +1933,18 @@
         <v>102</v>
       </c>
       <c r="F59">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
@@ -1953,18 +1953,18 @@
         <v>102</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
       <c r="C61" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
@@ -1973,58 +1973,58 @@
         <v>102</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
       </c>
       <c r="E62" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="F62">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="B63" t="s">
-        <v>110</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
       </c>
       <c r="E63" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="F63">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D64" t="s">
         <v>6</v>
@@ -2033,18 +2033,18 @@
         <v>114</v>
       </c>
       <c r="F64">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D65" t="s">
         <v>6</v>
@@ -2053,46 +2053,6 @@
         <v>114</v>
       </c>
       <c r="F65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>116</v>
-      </c>
-      <c r="B66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" t="s">
-        <v>117</v>
-      </c>
-      <c r="D66" t="s">
-        <v>6</v>
-      </c>
-      <c r="E66" t="s">
-        <v>114</v>
-      </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>12</v>
-      </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" t="s">
-        <v>118</v>
-      </c>
-      <c r="D67" t="s">
-        <v>6</v>
-      </c>
-      <c r="E67" t="s">
-        <v>114</v>
-      </c>
-      <c r="F67">
         <v>2</v>
       </c>
     </row>

</xml_diff>